<commit_message>
update chiều 9/9 lần 1
</commit_message>
<xml_diff>
--- a/hoc_phi_full.xlsx
+++ b/hoc_phi_full.xlsx
@@ -50,28 +50,499 @@
     <t>Ghi chú</t>
   </si>
   <si>
+    <t>Bác sĩ Răng - Hàm - Mặt</t>
+  </si>
+  <si>
+    <t>304</t>
+  </si>
+  <si>
+    <t>Bác sĩ Đa khoa</t>
+  </si>
+  <si>
+    <t>305</t>
+  </si>
+  <si>
+    <t>Ngành Khoa học Máy tính (TROY)</t>
+  </si>
+  <si>
+    <t>102(TROY)</t>
+  </si>
+  <si>
+    <t>Ngành Quản trị Kinh doanh (TROY)</t>
+  </si>
+  <si>
+    <t>400(TROY)</t>
+  </si>
+  <si>
+    <t>Ngành Quản trị Khách sạn (TROY)</t>
+  </si>
+  <si>
+    <t>407(TROY)</t>
+  </si>
+  <si>
+    <t>Thiết kế Đồ họa</t>
+  </si>
+  <si>
+    <t>111(VJJ)</t>
+  </si>
+  <si>
+    <t>Công nghệ Kỹ thuật Ô tô</t>
+  </si>
+  <si>
+    <t>117(VJJ)</t>
+  </si>
+  <si>
+    <t>Quản trị Khách sạn Quốc tế (PSU)</t>
+  </si>
+  <si>
+    <t>414(PSU)</t>
+  </si>
+  <si>
+    <t>Quản trị Du lịch &amp; Dịch vụ Hàng không</t>
+  </si>
+  <si>
+    <t>444</t>
+  </si>
+  <si>
+    <t>Logistics &amp; Quản lý Chuỗi cung ứng (HP)</t>
+  </si>
+  <si>
+    <t>416(HP)</t>
+  </si>
+  <si>
+    <t>Mạng Máy tính và Truyền thông Dữ liệu</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>Công nghệ Phần mềm</t>
+  </si>
+  <si>
+    <t>102(VJJ)</t>
+  </si>
+  <si>
+    <t>Quản trị Du lịch &amp; Lữ hành chuẩn PSU</t>
+  </si>
+  <si>
+    <t>408(PSU)</t>
+  </si>
+  <si>
+    <t>Công nghệ phần mềm chuẩn CMU (Đạt kiểm định ABET)</t>
+  </si>
+  <si>
+    <t>102(CMU)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digital Marketing </t>
+  </si>
+  <si>
+    <t>Logistics &amp; Quản lý Chuỗi Cung Ứng</t>
+  </si>
+  <si>
+    <t>416</t>
+  </si>
+  <si>
+    <t>Dược sĩ (Đại học)</t>
+  </si>
+  <si>
+    <t>303</t>
+  </si>
+  <si>
+    <t>Y học Cổ truyền</t>
+  </si>
+  <si>
+    <t>325</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>Thiết kế Mỹ thuật số</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>Quản trị Sự kiện &amp; Giải trí</t>
+  </si>
+  <si>
+    <t>413</t>
+  </si>
+  <si>
+    <t>Truyền thông Đa phương tiện</t>
+  </si>
+  <si>
+    <t>607</t>
+  </si>
+  <si>
+    <t>Quan hệ Công chúng</t>
+  </si>
+  <si>
+    <t>610</t>
+  </si>
+  <si>
+    <t>Tiếng Trung Biên - Phiên dịch</t>
+  </si>
+  <si>
+    <t>703</t>
+  </si>
+  <si>
+    <t>An ninh mạng chuẩn CMU</t>
+  </si>
+  <si>
+    <t>116(CMU)</t>
+  </si>
+  <si>
+    <t>Quản trị Kinh doanh chuẩn PSU</t>
+  </si>
+  <si>
+    <t>400(PSU)</t>
+  </si>
+  <si>
+    <t>Quản trị Marketing &amp; Chiến lược (HP)</t>
+  </si>
+  <si>
+    <t>401(HP)</t>
+  </si>
+  <si>
+    <t>Công nghệ Phần mềm (Đạt kiểm định ABET)</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>Kỹ thuật Điều khiển &amp; Tự động hóa</t>
+  </si>
+  <si>
+    <t>118(VJJ)</t>
+  </si>
+  <si>
     <t>Quản trị Du lịch &amp; Lữ hành</t>
   </si>
   <si>
     <t>408</t>
   </si>
   <si>
-    <t>Quản trị Du lịch &amp; Lữ hành chuẩn PSU</t>
-  </si>
-  <si>
-    <t>408(PSU)</t>
-  </si>
-  <si>
     <t>Quản trị Du lịch &amp; Khách Sạn</t>
   </si>
   <si>
     <t>407</t>
   </si>
   <si>
-    <t>Quản trị Sự kiện &amp; Giải trí</t>
-  </si>
-  <si>
-    <t>413</t>
+    <t>Quản trị Nhà hàng Quốc tế (PSU)</t>
+  </si>
+  <si>
+    <t>425(PSU)</t>
+  </si>
+  <si>
+    <t>Quản trị Kinh doanh Marketing</t>
+  </si>
+  <si>
+    <t>401</t>
+  </si>
+  <si>
+    <t>Công nghệ Tài chính (Fintech)</t>
+  </si>
+  <si>
+    <t>435</t>
+  </si>
+  <si>
+    <t>Thiết kế Games và Multimedia</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>Khoa học Máy tính</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>Luật Kinh doanh (HP)</t>
+  </si>
+  <si>
+    <t>609(HP)</t>
+  </si>
+  <si>
+    <t>Tiếng Trung Thương mại</t>
+  </si>
+  <si>
+    <t>803</t>
+  </si>
+  <si>
+    <t>Tài chính - Ngân hàng chuẩn PSU</t>
+  </si>
+  <si>
+    <t>404(PSU)</t>
+  </si>
+  <si>
+    <t>Kế toán Kiểm toán chuẩn PSU</t>
+  </si>
+  <si>
+    <t>405(PSU)</t>
+  </si>
+  <si>
+    <t>Điện tử - Viễn thông</t>
+  </si>
+  <si>
+    <t>109(VJJ)</t>
+  </si>
+  <si>
+    <t>Quan hệ Quốc tế (HP)</t>
+  </si>
+  <si>
+    <t>608(HP)</t>
+  </si>
+  <si>
+    <t>Tiếng Anh Biên - Phiên dịch</t>
+  </si>
+  <si>
+    <t>701</t>
+  </si>
+  <si>
+    <t>Tiếng Nhật Biên - Phiên dịch</t>
+  </si>
+  <si>
+    <t>704</t>
+  </si>
+  <si>
+    <t>Tiếng Hàn Biên - Phiên dịch</t>
+  </si>
+  <si>
+    <t>705</t>
+  </si>
+  <si>
+    <t>Tiếng Trung Du lịch</t>
+  </si>
+  <si>
+    <t>707</t>
+  </si>
+  <si>
+    <t>Tiếng Anh Thương mại</t>
+  </si>
+  <si>
+    <t>801</t>
+  </si>
+  <si>
+    <t>Hệ thống Thông tin Quản lý chuẩn CMU (Đạt kiểm định ABET)</t>
+  </si>
+  <si>
+    <t>410(CMU)</t>
+  </si>
+  <si>
+    <t>Xét nghiệm Y học</t>
+  </si>
+  <si>
+    <t>330</t>
+  </si>
+  <si>
+    <t>Quản trị Doanh nghiệp (HP)</t>
+  </si>
+  <si>
+    <t>400(HP)</t>
+  </si>
+  <si>
+    <t>Quản trị Tài chính (HP)</t>
+  </si>
+  <si>
+    <t>403(HP)</t>
+  </si>
+  <si>
+    <t>Cơ điện tử chuẩn PNU</t>
+  </si>
+  <si>
+    <t>112(PNU)</t>
+  </si>
+  <si>
+    <t>Điện - Điện tử chuẩn PNU</t>
+  </si>
+  <si>
+    <t>113(PNU)</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>Thiết kế Thời trang</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>Công nghệ Chế tạo Máy</t>
+  </si>
+  <si>
+    <t>Thiết kế Vi Mạch Bán dẫn</t>
+  </si>
+  <si>
+    <t>Điện Cơ Ô tô</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>Kỹ thuật Mạng (Đạt kiểm định ABET)</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>Trí tuệ Nhân tạo (HP)</t>
+  </si>
+  <si>
+    <t>121(HP)</t>
+  </si>
+  <si>
+    <t>An toàn Thông tin</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>Công nghệ Thực phẩm</t>
+  </si>
+  <si>
+    <t>306(VJJ)</t>
+  </si>
+  <si>
+    <t>Điều dưỡng Đa khoa</t>
+  </si>
+  <si>
+    <t>302(VJJ)</t>
+  </si>
+  <si>
+    <t>Quản trị Kinh doanh Tổng hợp</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>Kế toán Quản trị (HP)</t>
+  </si>
+  <si>
+    <t>406(HP)</t>
+  </si>
+  <si>
+    <t>Thương mại Điện tử</t>
+  </si>
+  <si>
+    <t>422</t>
+  </si>
+  <si>
+    <t>Phân tích Kinh doanh (Business Analytics)</t>
+  </si>
+  <si>
+    <t>427</t>
+  </si>
+  <si>
+    <t>Luật học</t>
+  </si>
+  <si>
+    <t>606</t>
+  </si>
+  <si>
+    <t>Luật Kinh tế</t>
+  </si>
+  <si>
+    <t>609</t>
+  </si>
+  <si>
+    <t>Big Data &amp; Machine Learning (HP)</t>
+  </si>
+  <si>
+    <t>115(HP)</t>
+  </si>
+  <si>
+    <t>Kỹ thuật máy tính</t>
+  </si>
+  <si>
+    <t>Khoa học Dữ liệu</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>Kinh doanh Thương mại</t>
+  </si>
+  <si>
+    <t>412</t>
+  </si>
+  <si>
+    <t>Quản trị Kinh doanh Quốc tế (Ngoại Thương)</t>
+  </si>
+  <si>
+    <t>411</t>
+  </si>
+  <si>
+    <t>Tiếng Anh Du lịch</t>
+  </si>
+  <si>
+    <t>702</t>
+  </si>
+  <si>
+    <t>Tiếng Hàn Du lịch</t>
+  </si>
+  <si>
+    <t>706</t>
+  </si>
+  <si>
+    <t>Tiếng Nhật Du lịch</t>
+  </si>
+  <si>
+    <t>708</t>
+  </si>
+  <si>
+    <t>Tiếng Nhật Thương mại</t>
+  </si>
+  <si>
+    <t>804</t>
+  </si>
+  <si>
+    <t>Tiếng Hàn Thương mại</t>
+  </si>
+  <si>
+    <t>805</t>
+  </si>
+  <si>
+    <t>Kỹ thuật Điện</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Kinh tế Đầu tư</t>
+  </si>
+  <si>
+    <t>433</t>
+  </si>
+  <si>
+    <t>Kinh tế Quốc tế</t>
+  </si>
+  <si>
+    <t>418</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>Điện Tự động</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>Xây dựng Dân dụng &amp; Công nghiệp</t>
+  </si>
+  <si>
+    <t>105(VJJ)</t>
+  </si>
+  <si>
+    <t>Đã giảm 30%</t>
   </si>
   <si>
     <t>Smart Tourism (Du lịch thông minh)</t>
@@ -80,18 +551,6 @@
     <t>445</t>
   </si>
   <si>
-    <t>Quản trị Khách sạn Quốc tế (PSU)</t>
-  </si>
-  <si>
-    <t>414(PSU)</t>
-  </si>
-  <si>
-    <t>Quản trị Nhà hàng Quốc tế (PSU)</t>
-  </si>
-  <si>
-    <t>425(PSU)</t>
-  </si>
-  <si>
     <t>Hướng dẫn Du lịch Quốc tế (tiếng Anh)</t>
   </si>
   <si>
@@ -110,33 +569,12 @@
     <t>442</t>
   </si>
   <si>
-    <t>Quản trị Du lịch &amp; Dịch vụ Hàng không</t>
-  </si>
-  <si>
-    <t>444</t>
-  </si>
-  <si>
     <t>Quản lý &amp; Khởi sự Doanh nghiệp Nhỏ &amp; Vừa (SME)</t>
   </si>
   <si>
     <t>446</t>
   </si>
   <si>
-    <t>Quản trị Kinh doanh Tổng hợp</t>
-  </si>
-  <si>
-    <t>400</t>
-  </si>
-  <si>
-    <t>Quản trị Kinh doanh Marketing</t>
-  </si>
-  <si>
-    <t>401</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digital Marketing </t>
-  </si>
-  <si>
     <t>Tài chính Doanh nghiệp</t>
   </si>
   <si>
@@ -161,30 +599,6 @@
     <t>406</t>
   </si>
   <si>
-    <t>Kế toán Quản trị (HP)</t>
-  </si>
-  <si>
-    <t>406(HP)</t>
-  </si>
-  <si>
-    <t>Kinh doanh Thương mại</t>
-  </si>
-  <si>
-    <t>412</t>
-  </si>
-  <si>
-    <t>Quản trị Kinh doanh Quốc tế (Ngoại Thương)</t>
-  </si>
-  <si>
-    <t>411</t>
-  </si>
-  <si>
-    <t>Logistics &amp; Quản lý Chuỗi Cung Ứng</t>
-  </si>
-  <si>
-    <t>416</t>
-  </si>
-  <si>
     <t>Quản trị Nhân lực</t>
   </si>
   <si>
@@ -197,34 +611,37 @@
     <t>415</t>
   </si>
   <si>
-    <t>Thương mại Điện tử</t>
-  </si>
-  <si>
-    <t>422</t>
-  </si>
-  <si>
-    <t>Kinh tế Đầu tư</t>
-  </si>
-  <si>
-    <t>433</t>
-  </si>
-  <si>
-    <t>Công nghệ Tài chính (Fintech)</t>
-  </si>
-  <si>
-    <t>435</t>
-  </si>
-  <si>
-    <t>Phân tích Kinh doanh (Business Analytics)</t>
-  </si>
-  <si>
-    <t>427</t>
-  </si>
-  <si>
-    <t>Kinh tế Quốc tế</t>
-  </si>
-  <si>
-    <t>418</t>
+    <t>Quan hệ Quốc tế (Chương trình Tiếng Anh)</t>
+  </si>
+  <si>
+    <t>608</t>
+  </si>
+  <si>
+    <t>Công nghệ Thực phẩm (Đạt kiểm định ABET)</t>
+  </si>
+  <si>
+    <t>306</t>
+  </si>
+  <si>
+    <t>302</t>
+  </si>
+  <si>
+    <t>Công nghệ Sinh học</t>
+  </si>
+  <si>
+    <t>310</t>
+  </si>
+  <si>
+    <t>Kỹ thuật Y sinh</t>
+  </si>
+  <si>
+    <t>320</t>
+  </si>
+  <si>
+    <t>Kiến trúc Công trình</t>
+  </si>
+  <si>
+    <t>107(VJJ)</t>
   </si>
   <si>
     <t>Việt Nam học</t>
@@ -239,132 +656,6 @@
     <t>601</t>
   </si>
   <si>
-    <t>Luật học</t>
-  </si>
-  <si>
-    <t>606</t>
-  </si>
-  <si>
-    <t>Truyền thông Đa phương tiện</t>
-  </si>
-  <si>
-    <t>607</t>
-  </si>
-  <si>
-    <t>Quan hệ Quốc tế (Chương trình Tiếng Anh)</t>
-  </si>
-  <si>
-    <t>608</t>
-  </si>
-  <si>
-    <t>Quan hệ Quốc tế (HP)</t>
-  </si>
-  <si>
-    <t>608(HP)</t>
-  </si>
-  <si>
-    <t>Luật Kinh tế</t>
-  </si>
-  <si>
-    <t>609</t>
-  </si>
-  <si>
-    <t>Luật Kinh doanh (HP)</t>
-  </si>
-  <si>
-    <t>609(HP)</t>
-  </si>
-  <si>
-    <t>Quan hệ Công chúng</t>
-  </si>
-  <si>
-    <t>610</t>
-  </si>
-  <si>
-    <t>Tiếng Anh Biên - Phiên dịch</t>
-  </si>
-  <si>
-    <t>701</t>
-  </si>
-  <si>
-    <t>Tiếng Anh Du lịch</t>
-  </si>
-  <si>
-    <t>702</t>
-  </si>
-  <si>
-    <t>Tiếng Trung Biên - Phiên dịch</t>
-  </si>
-  <si>
-    <t>703</t>
-  </si>
-  <si>
-    <t>Tiếng Nhật Biên - Phiên dịch</t>
-  </si>
-  <si>
-    <t>704</t>
-  </si>
-  <si>
-    <t>Tiếng Hàn Biên - Phiên dịch</t>
-  </si>
-  <si>
-    <t>705</t>
-  </si>
-  <si>
-    <t>Tiếng Hàn Du lịch</t>
-  </si>
-  <si>
-    <t>706</t>
-  </si>
-  <si>
-    <t>Tiếng Trung Du lịch</t>
-  </si>
-  <si>
-    <t>707</t>
-  </si>
-  <si>
-    <t>Tiếng Nhật Du lịch</t>
-  </si>
-  <si>
-    <t>708</t>
-  </si>
-  <si>
-    <t>Tiếng Anh Thương mại</t>
-  </si>
-  <si>
-    <t>801</t>
-  </si>
-  <si>
-    <t>Tiếng Trung Thương mại</t>
-  </si>
-  <si>
-    <t>803</t>
-  </si>
-  <si>
-    <t>Tiếng Nhật Thương mại</t>
-  </si>
-  <si>
-    <t>804</t>
-  </si>
-  <si>
-    <t>Tiếng Hàn Thương mại</t>
-  </si>
-  <si>
-    <t>805</t>
-  </si>
-  <si>
-    <t>An ninh mạng chuẩn CMU</t>
-  </si>
-  <si>
-    <t>116(CMU)</t>
-  </si>
-  <si>
-    <t>Công nghệ phần mềm chuẩn CMU (Đạt kiểm định ABET)</t>
-  </si>
-  <si>
-    <t>102(CMU)</t>
-  </si>
-  <si>
     <t>Xây dựng Dân dụng &amp; Công nghiệp chuẩn CSU</t>
   </si>
   <si>
@@ -380,156 +671,6 @@
     <t>107(CSU)</t>
   </si>
   <si>
-    <t>Quản trị Kinh doanh chuẩn PSU</t>
-  </si>
-  <si>
-    <t>400(PSU)</t>
-  </si>
-  <si>
-    <t>Tài chính - Ngân hàng chuẩn PSU</t>
-  </si>
-  <si>
-    <t>404(PSU)</t>
-  </si>
-  <si>
-    <t>Kế toán Kiểm toán chuẩn PSU</t>
-  </si>
-  <si>
-    <t>405(PSU)</t>
-  </si>
-  <si>
-    <t>Hệ thống Thông tin Quản lý chuẩn CMU (Đạt kiểm định ABET)</t>
-  </si>
-  <si>
-    <t>410(CMU)</t>
-  </si>
-  <si>
-    <t>Điều dưỡng Đa khoa</t>
-  </si>
-  <si>
-    <t>302</t>
-  </si>
-  <si>
-    <t>Dược sĩ (Đại học)</t>
-  </si>
-  <si>
-    <t>303</t>
-  </si>
-  <si>
-    <t>Bác sĩ Răng - Hàm - Mặt</t>
-  </si>
-  <si>
-    <t>304</t>
-  </si>
-  <si>
-    <t>Bác sĩ Đa khoa</t>
-  </si>
-  <si>
-    <t>305</t>
-  </si>
-  <si>
-    <t>Công nghệ Sinh học</t>
-  </si>
-  <si>
-    <t>310</t>
-  </si>
-  <si>
-    <t>Đã giảm 30%</t>
-  </si>
-  <si>
-    <t>Kỹ thuật Y sinh</t>
-  </si>
-  <si>
-    <t>320</t>
-  </si>
-  <si>
-    <t>Y học Cổ truyền</t>
-  </si>
-  <si>
-    <t>325</t>
-  </si>
-  <si>
-    <t>Xét nghiệm Y học</t>
-  </si>
-  <si>
-    <t>330</t>
-  </si>
-  <si>
-    <t>Logistics &amp; Quản lý Chuỗi cung ứng (HP)</t>
-  </si>
-  <si>
-    <t>416(HP)</t>
-  </si>
-  <si>
-    <t>Quản trị Doanh nghiệp (HP)</t>
-  </si>
-  <si>
-    <t>400(HP)</t>
-  </si>
-  <si>
-    <t>Quản trị Marketing &amp; Chiến lược (HP)</t>
-  </si>
-  <si>
-    <t>401(HP)</t>
-  </si>
-  <si>
-    <t>Quản trị Tài chính (HP)</t>
-  </si>
-  <si>
-    <t>403(HP)</t>
-  </si>
-  <si>
-    <t>Công nghệ Phần mềm</t>
-  </si>
-  <si>
-    <t>102(VJJ)</t>
-  </si>
-  <si>
-    <t>Xây dựng Dân dụng &amp; Công nghiệp</t>
-  </si>
-  <si>
-    <t>105(VJJ)</t>
-  </si>
-  <si>
-    <t>Kiến trúc Công trình</t>
-  </si>
-  <si>
-    <t>107(VJJ)</t>
-  </si>
-  <si>
-    <t>Điện tử - Viễn thông</t>
-  </si>
-  <si>
-    <t>109(VJJ)</t>
-  </si>
-  <si>
-    <t>Thiết kế Đồ họa</t>
-  </si>
-  <si>
-    <t>111(VJJ)</t>
-  </si>
-  <si>
-    <t>Công nghệ Kỹ thuật Ô tô</t>
-  </si>
-  <si>
-    <t>117(VJJ)</t>
-  </si>
-  <si>
-    <t>Kỹ thuật Điều khiển &amp; Tự động hóa</t>
-  </si>
-  <si>
-    <t>118(VJJ)</t>
-  </si>
-  <si>
-    <t>302(VJJ)</t>
-  </si>
-  <si>
-    <t>Công nghệ Thực phẩm</t>
-  </si>
-  <si>
-    <t>306(VJJ)</t>
-  </si>
-  <si>
     <t>105</t>
   </si>
   <si>
@@ -542,84 +683,18 @@
     <t>107</t>
   </si>
   <si>
-    <t>109</t>
-  </si>
-  <si>
-    <t>Điện Tự động</t>
-  </si>
-  <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>111</t>
-  </si>
-  <si>
-    <t>Thiết kế Mỹ thuật số</t>
-  </si>
-  <si>
-    <t>129</t>
-  </si>
-  <si>
-    <t>Cơ điện tử chuẩn PNU</t>
-  </si>
-  <si>
-    <t>112(PNU)</t>
-  </si>
-  <si>
-    <t>Điện - Điện tử chuẩn PNU</t>
-  </si>
-  <si>
-    <t>113(PNU)</t>
-  </si>
-  <si>
-    <t>117</t>
-  </si>
-  <si>
-    <t>118</t>
-  </si>
-  <si>
-    <t>Thiết kế Thời trang</t>
-  </si>
-  <si>
-    <t>119</t>
-  </si>
-  <si>
     <t>Thiết kế Nội thất</t>
   </si>
   <si>
     <t>123</t>
   </si>
   <si>
-    <t>Công nghệ Chế tạo Máy</t>
-  </si>
-  <si>
-    <t>Thiết kế Vi Mạch Bán dẫn</t>
-  </si>
-  <si>
-    <t>Điện Cơ Ô tô</t>
-  </si>
-  <si>
-    <t>145</t>
-  </si>
-  <si>
-    <t>Kỹ thuật Điện</t>
-  </si>
-  <si>
-    <t>150</t>
-  </si>
-  <si>
     <t>Công nghệ Quản lý Xây dựng</t>
   </si>
   <si>
     <t>206</t>
   </si>
   <si>
-    <t>Công nghệ Thực phẩm (Đạt kiểm định ABET)</t>
-  </si>
-  <si>
-    <t>306</t>
-  </si>
-  <si>
     <t>Công nghệ &amp; Kỹ thuật Môi trường</t>
   </si>
   <si>
@@ -630,81 +705,6 @@
   </si>
   <si>
     <t>307</t>
-  </si>
-  <si>
-    <t>Kỹ thuật Mạng (Đạt kiểm định ABET)</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>Công nghệ Phần mềm (Đạt kiểm định ABET)</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>Big Data &amp; Machine Learning (HP)</t>
-  </si>
-  <si>
-    <t>115(HP)</t>
-  </si>
-  <si>
-    <t>Trí tuệ Nhân tạo (HP)</t>
-  </si>
-  <si>
-    <t>121(HP)</t>
-  </si>
-  <si>
-    <t>Thiết kế Games và Multimedia</t>
-  </si>
-  <si>
-    <t>122</t>
-  </si>
-  <si>
-    <t>An toàn Thông tin</t>
-  </si>
-  <si>
-    <t>124</t>
-  </si>
-  <si>
-    <t>Kỹ thuật máy tính</t>
-  </si>
-  <si>
-    <t>Khoa học Máy tính</t>
-  </si>
-  <si>
-    <t>130</t>
-  </si>
-  <si>
-    <t>Khoa học Dữ liệu</t>
-  </si>
-  <si>
-    <t>135</t>
-  </si>
-  <si>
-    <t>Mạng Máy tính và Truyền thông Dữ liệu</t>
-  </si>
-  <si>
-    <t>140</t>
-  </si>
-  <si>
-    <t>Ngành Khoa học Máy tính (TROY)</t>
-  </si>
-  <si>
-    <t>102(TROY)</t>
-  </si>
-  <si>
-    <t>Ngành Quản trị Kinh doanh (TROY)</t>
-  </si>
-  <si>
-    <t>400(TROY)</t>
-  </si>
-  <si>
-    <t>Ngành Quản trị Khách sạn (TROY)</t>
-  </si>
-  <si>
-    <t>407(TROY)</t>
   </si>
 </sst>
 </file>
@@ -1346,10 +1346,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1699,8 +1699,8 @@
   <sheetPr/>
   <dimension ref="A1:H120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
-      <selection activeCell="A112" sqref="A112:A115"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="7"/>
@@ -1738,7 +1738,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>1</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1747,18 +1747,18 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>1035000</v>
+        <v>3090000</v>
       </c>
       <c r="E2">
-        <v>16560000</v>
+        <v>49200000</v>
       </c>
       <c r="F2">
-        <v>33120000</v>
+        <v>98880000</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -1767,78 +1767,72 @@
         <v>10</v>
       </c>
       <c r="D3">
-        <v>1200000</v>
+        <v>2950000</v>
       </c>
       <c r="E3">
-        <v>19200000</v>
+        <v>47200000</v>
       </c>
       <c r="F3">
-        <v>38400000</v>
+        <v>94400000</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
-        <v>1035000</v>
-      </c>
+      <c r="D4" s="2"/>
       <c r="E4">
-        <v>16560000</v>
-      </c>
-      <c r="F4">
-        <v>33120000</v>
+        <v>32000000</v>
+      </c>
+      <c r="F4" s="2">
+        <v>64000000</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D5">
-        <v>1100000</v>
-      </c>
+      <c r="D5" s="2"/>
       <c r="E5">
-        <v>17600000</v>
-      </c>
-      <c r="F5">
-        <v>35200000</v>
+        <v>32000000</v>
+      </c>
+      <c r="F5" s="2">
+        <v>64000000</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6">
-        <v>785000</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6">
-        <v>12560000</v>
-      </c>
-      <c r="F6">
-        <v>25120000</v>
+        <v>32000000</v>
+      </c>
+      <c r="F6" s="2">
+        <v>64000000</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>6</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -1847,18 +1841,18 @@
         <v>18</v>
       </c>
       <c r="D7">
-        <v>1250000</v>
+        <v>1280000</v>
       </c>
       <c r="E7">
-        <v>20000000</v>
+        <v>20480000</v>
       </c>
       <c r="F7">
-        <v>40000000</v>
+        <v>40960000</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
@@ -1867,18 +1861,18 @@
         <v>20</v>
       </c>
       <c r="D8">
-        <v>1035000</v>
+        <v>1280000</v>
       </c>
       <c r="E8">
-        <v>16560000</v>
+        <v>20480000</v>
       </c>
       <c r="F8">
-        <v>33120000</v>
+        <v>40960000</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
@@ -1887,18 +1881,18 @@
         <v>22</v>
       </c>
       <c r="D9">
-        <v>785000</v>
+        <v>1250000</v>
       </c>
       <c r="E9">
-        <v>12560000</v>
+        <v>20000000</v>
       </c>
       <c r="F9">
-        <v>25120000</v>
+        <v>40000000</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -1907,18 +1901,18 @@
         <v>24</v>
       </c>
       <c r="D10">
-        <v>785000</v>
+        <v>1250000</v>
       </c>
       <c r="E10">
-        <v>12560000</v>
+        <v>20000000</v>
       </c>
       <c r="F10">
-        <v>25120000</v>
+        <v>40000000</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
         <v>25</v>
@@ -1927,18 +1921,18 @@
         <v>26</v>
       </c>
       <c r="D11">
-        <v>785000</v>
+        <v>1250000</v>
       </c>
       <c r="E11">
-        <v>12560000</v>
+        <v>20000000</v>
       </c>
       <c r="F11">
-        <v>25120000</v>
+        <v>40000000</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
         <v>27</v>
@@ -1952,13 +1946,13 @@
       <c r="E12">
         <v>20000000</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="3">
         <v>40000000</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="A13">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
@@ -1967,18 +1961,18 @@
         <v>30</v>
       </c>
       <c r="D13">
-        <v>785000</v>
+        <v>1225000</v>
       </c>
       <c r="E13">
-        <v>12560000</v>
+        <v>19600000</v>
       </c>
       <c r="F13">
-        <v>25120000</v>
+        <v>39200000</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
         <v>31</v>
@@ -1987,18 +1981,18 @@
         <v>32</v>
       </c>
       <c r="D14">
-        <v>875000</v>
+        <v>1200000</v>
       </c>
       <c r="E14">
-        <v>14000000</v>
+        <v>19200000</v>
       </c>
       <c r="F14">
-        <v>28000000</v>
+        <v>38400000</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
         <v>33</v>
@@ -2007,13 +2001,13 @@
         <v>34</v>
       </c>
       <c r="D15">
-        <v>1035000</v>
+        <v>1200000</v>
       </c>
       <c r="E15">
-        <v>16560000</v>
+        <v>19200000</v>
       </c>
       <c r="F15">
-        <v>33120000</v>
+        <v>38400000</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2038,7 +2032,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -2047,18 +2041,18 @@
         <v>37</v>
       </c>
       <c r="D17">
-        <v>785000</v>
+        <v>1155000</v>
       </c>
       <c r="E17">
-        <v>12560000</v>
+        <v>18480000</v>
       </c>
       <c r="F17">
-        <v>25120000</v>
+        <v>36960000</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
         <v>38</v>
@@ -2067,18 +2061,18 @@
         <v>39</v>
       </c>
       <c r="D18">
-        <v>785000</v>
+        <v>1155000</v>
       </c>
       <c r="E18">
-        <v>12560000</v>
+        <v>18480000</v>
       </c>
       <c r="F18">
-        <v>25120000</v>
+        <v>36960000</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19">
-        <v>18</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
         <v>40</v>
@@ -2087,393 +2081,393 @@
         <v>41</v>
       </c>
       <c r="D19">
-        <v>785000</v>
+        <v>1155000</v>
       </c>
       <c r="E19">
-        <v>12560000</v>
+        <v>18480000</v>
       </c>
       <c r="F19">
-        <v>25120000</v>
+        <v>36960000</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="B20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" t="s">
         <v>42</v>
       </c>
-      <c r="C20" t="s">
-        <v>43</v>
-      </c>
       <c r="D20">
-        <v>785000</v>
+        <v>1155000</v>
       </c>
       <c r="E20">
-        <v>12560000</v>
+        <v>18480000</v>
       </c>
       <c r="F20">
-        <v>25120000</v>
+        <v>36960000</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="B21" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" t="s">
         <v>44</v>
       </c>
-      <c r="C21" t="s">
-        <v>45</v>
-      </c>
       <c r="D21">
-        <v>875000</v>
+        <v>1155000</v>
       </c>
       <c r="E21">
-        <v>14000000</v>
+        <v>18480000</v>
       </c>
       <c r="F21">
-        <v>28000000</v>
+        <v>36960000</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22">
-        <v>845000</v>
+        <v>1155000</v>
       </c>
       <c r="E22">
-        <v>13520000</v>
+        <v>18480000</v>
       </c>
       <c r="F22">
-        <v>27040000</v>
+        <v>36960000</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D23">
-        <v>845000</v>
+        <v>1100000</v>
       </c>
       <c r="E23">
-        <v>13520000</v>
+        <v>17600000</v>
       </c>
       <c r="F23">
-        <v>27040000</v>
+        <v>35200000</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D24">
-        <v>1155000</v>
+        <v>1100000</v>
       </c>
       <c r="E24">
-        <v>18480000</v>
+        <v>17600000</v>
       </c>
       <c r="F24">
-        <v>36960000</v>
+        <v>35200000</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D25">
-        <v>785000</v>
+        <v>1100000</v>
       </c>
       <c r="E25">
-        <v>12560000</v>
+        <v>17600000</v>
       </c>
       <c r="F25">
-        <v>25120000</v>
+        <v>35200000</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D26">
-        <v>785000</v>
+        <v>1100000</v>
       </c>
       <c r="E26">
-        <v>12560000</v>
+        <v>17600000</v>
       </c>
       <c r="F26">
-        <v>25120000</v>
+        <v>35200000</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D27">
-        <v>875000</v>
+        <v>1100000</v>
       </c>
       <c r="E27">
-        <v>14000000</v>
+        <v>17600000</v>
       </c>
       <c r="F27">
-        <v>28000000</v>
+        <v>35200000</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D28">
-        <v>825000</v>
+        <v>1100000</v>
       </c>
       <c r="E28">
-        <v>13200000</v>
+        <v>17600000</v>
       </c>
       <c r="F28">
-        <v>26400000</v>
+        <v>35200000</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29">
-        <v>28</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D29">
-        <v>1035000</v>
+        <v>1100000</v>
       </c>
       <c r="E29">
-        <v>16560000</v>
+        <v>17600000</v>
       </c>
       <c r="F29">
-        <v>33120000</v>
+        <v>35200000</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="B30" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D30">
-        <v>875000</v>
+        <v>1100000</v>
       </c>
       <c r="E30">
-        <v>14000000</v>
+        <v>17600000</v>
       </c>
       <c r="F30">
-        <v>28000000</v>
+        <v>35200000</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31">
-        <v>30</v>
+        <v>78</v>
       </c>
       <c r="B31" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C31" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D31">
-        <v>825000</v>
+        <v>1065000</v>
       </c>
       <c r="E31">
-        <v>13200000</v>
+        <v>17040000</v>
       </c>
       <c r="F31">
-        <v>26400000</v>
+        <v>34080000</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D32">
-        <v>700000</v>
+        <v>1035000</v>
       </c>
       <c r="E32">
-        <v>11200000</v>
+        <v>16560000</v>
       </c>
       <c r="F32">
-        <v>22400000</v>
+        <v>33120000</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="B33" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D33">
-        <v>700000</v>
+        <v>1035000</v>
       </c>
       <c r="E33">
-        <v>11200000</v>
+        <v>16560000</v>
       </c>
       <c r="F33">
-        <v>22400000</v>
+        <v>33120000</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D34">
-        <v>875000</v>
+        <v>1035000</v>
       </c>
       <c r="E34">
-        <v>14000000</v>
+        <v>16560000</v>
       </c>
       <c r="F34">
-        <v>28000000</v>
+        <v>33120000</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B35" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C35" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D35">
-        <v>1100000</v>
+        <v>1035000</v>
       </c>
       <c r="E35">
-        <v>17600000</v>
+        <v>16560000</v>
       </c>
       <c r="F35">
-        <v>35200000</v>
+        <v>33120000</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D36">
-        <v>785000</v>
+        <v>1035000</v>
       </c>
       <c r="E36">
-        <v>12560000</v>
+        <v>16560000</v>
       </c>
       <c r="F36">
-        <v>25120000</v>
+        <v>33120000</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37">
-        <v>36</v>
+        <v>106</v>
       </c>
       <c r="B37" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D37">
-        <v>940000</v>
+        <v>1035000</v>
       </c>
       <c r="E37">
-        <v>15040000</v>
+        <v>16560000</v>
       </c>
       <c r="F37">
-        <v>30080000</v>
+        <v>33120000</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="B38" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D38">
-        <v>875000</v>
+        <v>1035000</v>
       </c>
       <c r="E38">
-        <v>14000000</v>
+        <v>16560000</v>
       </c>
       <c r="F38">
-        <v>28000000</v>
+        <v>33120000</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -2481,10 +2475,10 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D39">
         <v>1000000</v>
@@ -2498,93 +2492,93 @@
     </row>
     <row r="40" spans="1:6">
       <c r="A40">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D40">
-        <v>1100000</v>
+        <v>1000000</v>
       </c>
       <c r="E40">
-        <v>17600000</v>
+        <v>16000000</v>
       </c>
       <c r="F40">
-        <v>35200000</v>
+        <v>32000000</v>
       </c>
     </row>
     <row r="41" spans="1:6">
       <c r="A41">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D41">
-        <v>940000</v>
+        <v>1000000</v>
       </c>
       <c r="E41">
-        <v>15040000</v>
+        <v>16000000</v>
       </c>
       <c r="F41">
-        <v>30080000</v>
+        <v>32000000</v>
       </c>
     </row>
     <row r="42" spans="1:6">
       <c r="A42">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B42" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C42" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D42">
-        <v>845000</v>
+        <v>1000000</v>
       </c>
       <c r="E42">
-        <v>13520000</v>
+        <v>16000000</v>
       </c>
       <c r="F42">
-        <v>27040000</v>
+        <v>32000000</v>
       </c>
     </row>
     <row r="43" spans="1:6">
       <c r="A43">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D43">
-        <v>1100000</v>
+        <v>950000</v>
       </c>
       <c r="E43">
-        <v>17600000</v>
+        <v>15200000</v>
       </c>
       <c r="F43">
-        <v>35200000</v>
+        <v>30400000</v>
       </c>
     </row>
     <row r="44" spans="1:6">
       <c r="A44">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C44" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D44">
         <v>940000</v>
@@ -2598,13 +2592,13 @@
     </row>
     <row r="45" spans="1:6">
       <c r="A45">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C45" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D45">
         <v>940000</v>
@@ -2618,33 +2612,33 @@
     </row>
     <row r="46" spans="1:6">
       <c r="A46">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C46" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D46">
-        <v>845000</v>
+        <v>940000</v>
       </c>
       <c r="E46">
-        <v>13520000</v>
+        <v>15040000</v>
       </c>
       <c r="F46">
-        <v>27040000</v>
+        <v>30080000</v>
       </c>
     </row>
     <row r="47" spans="1:6">
       <c r="A47">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C47" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D47">
         <v>940000</v>
@@ -2658,22 +2652,22 @@
     </row>
     <row r="48" spans="1:6">
       <c r="A48">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C48" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D48">
-        <v>845000</v>
+        <v>940000</v>
       </c>
       <c r="E48">
-        <v>13520000</v>
+        <v>15040000</v>
       </c>
       <c r="F48">
-        <v>27040000</v>
+        <v>30080000</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -2681,10 +2675,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C49" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D49">
         <v>940000</v>
@@ -2698,219 +2692,213 @@
     </row>
     <row r="50" spans="1:6">
       <c r="A50">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B50" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C50" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D50">
-        <v>1000000</v>
+        <v>940000</v>
       </c>
       <c r="E50">
-        <v>16000000</v>
+        <v>15040000</v>
       </c>
       <c r="F50">
-        <v>32000000</v>
+        <v>30080000</v>
       </c>
     </row>
     <row r="51" spans="1:6">
       <c r="A51">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="B51" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C51" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D51">
-        <v>845000</v>
+        <v>940000</v>
       </c>
       <c r="E51">
-        <v>13520000</v>
+        <v>15040000</v>
       </c>
       <c r="F51">
-        <v>27040000</v>
+        <v>30080000</v>
       </c>
     </row>
     <row r="52" spans="1:6">
       <c r="A52">
-        <v>51</v>
+        <v>69</v>
       </c>
       <c r="B52" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C52" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D52">
-        <v>845000</v>
+        <v>940000</v>
       </c>
       <c r="E52">
-        <v>13520000</v>
+        <v>15040000</v>
       </c>
       <c r="F52">
-        <v>27040000</v>
+        <v>30080000</v>
       </c>
     </row>
     <row r="53" spans="1:6">
       <c r="A53">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B53" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D53">
-        <v>1100000</v>
+        <v>940000</v>
       </c>
       <c r="E53">
-        <v>17600000</v>
+        <v>15040000</v>
       </c>
       <c r="F53">
-        <v>35200000</v>
+        <v>30080000</v>
       </c>
     </row>
     <row r="54" spans="1:6">
       <c r="A54">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="B54" t="s">
+        <v>108</v>
+      </c>
+      <c r="C54" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54">
+        <v>940000</v>
+      </c>
+      <c r="E54">
+        <v>15040000</v>
+      </c>
+      <c r="F54">
+        <v>30080000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55">
+        <v>89</v>
+      </c>
+      <c r="B55" t="s">
         <v>110</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>111</v>
       </c>
-      <c r="D54">
-        <v>1200000</v>
-      </c>
-      <c r="E54">
-        <v>19200000</v>
-      </c>
-      <c r="F54">
-        <v>38400000</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55">
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
+      <c r="D55">
+        <v>940000</v>
+      </c>
+      <c r="E55">
+        <v>15040000</v>
+      </c>
+      <c r="F55">
+        <v>30080000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56">
+        <v>91</v>
+      </c>
+      <c r="B56" t="s">
+        <v>62</v>
+      </c>
+      <c r="C56" t="s">
         <v>112</v>
       </c>
-      <c r="C55" t="s">
-        <v>113</v>
-      </c>
-      <c r="D55">
-        <v>680000</v>
-      </c>
-      <c r="E55">
-        <v>10880000</v>
-      </c>
-      <c r="F55">
-        <v>21760000</v>
-      </c>
-      <c r="G55" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7">
-      <c r="A56">
-        <v>55</v>
-      </c>
-      <c r="B56" t="s">
-        <v>115</v>
-      </c>
-      <c r="C56" t="s">
-        <v>116</v>
-      </c>
       <c r="D56">
-        <v>680000</v>
+        <v>940000</v>
       </c>
       <c r="E56">
-        <v>10880000</v>
+        <v>15040000</v>
       </c>
       <c r="F56">
-        <v>21760000</v>
-      </c>
-      <c r="G56" t="s">
-        <v>114</v>
+        <v>30080000</v>
       </c>
     </row>
     <row r="57" spans="1:6">
       <c r="A57">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="B57" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C57" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D57">
-        <v>1100000</v>
+        <v>940000</v>
       </c>
       <c r="E57">
-        <v>17600000</v>
+        <v>15040000</v>
       </c>
       <c r="F57">
-        <v>35200000</v>
+        <v>30080000</v>
       </c>
     </row>
     <row r="58" spans="1:6">
       <c r="A58">
-        <v>57</v>
+        <v>94</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
-      </c>
-      <c r="C58" t="s">
-        <v>120</v>
+        <v>115</v>
+      </c>
+      <c r="C58">
+        <v>125</v>
       </c>
       <c r="D58">
-        <v>1000000</v>
+        <v>940000</v>
       </c>
       <c r="E58">
-        <v>16000000</v>
+        <v>15040000</v>
       </c>
       <c r="F58">
-        <v>32000000</v>
+        <v>30080000</v>
       </c>
     </row>
     <row r="59" spans="1:6">
       <c r="A59">
-        <v>58</v>
+        <v>95</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
-      </c>
-      <c r="C59" t="s">
-        <v>122</v>
+        <v>116</v>
+      </c>
+      <c r="C59">
+        <v>127</v>
       </c>
       <c r="D59">
-        <v>1000000</v>
+        <v>940000</v>
       </c>
       <c r="E59">
-        <v>16000000</v>
+        <v>15040000</v>
       </c>
       <c r="F59">
-        <v>32000000</v>
+        <v>30080000</v>
       </c>
     </row>
     <row r="60" spans="1:6">
       <c r="A60">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C60" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D60">
         <v>940000</v>
@@ -2924,500 +2912,482 @@
     </row>
     <row r="61" spans="1:6">
       <c r="A61">
-        <v>60</v>
+        <v>102</v>
       </c>
       <c r="B61" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C61" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D61">
-        <v>770000</v>
+        <v>940000</v>
       </c>
       <c r="E61">
-        <v>12320000</v>
+        <v>15040000</v>
       </c>
       <c r="F61">
-        <v>24640000</v>
+        <v>30080000</v>
       </c>
     </row>
     <row r="62" spans="1:6">
       <c r="A62">
-        <v>61</v>
+        <v>105</v>
       </c>
       <c r="B62" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C62" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D62">
-        <v>1155000</v>
+        <v>940000</v>
       </c>
       <c r="E62">
-        <v>18480000</v>
+        <v>15040000</v>
       </c>
       <c r="F62">
-        <v>36960000</v>
+        <v>30080000</v>
       </c>
     </row>
     <row r="63" spans="1:6">
       <c r="A63">
-        <v>62</v>
+        <v>107</v>
       </c>
       <c r="B63" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C63" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="D63">
-        <v>3090000</v>
+        <v>940000</v>
       </c>
       <c r="E63">
-        <v>49200000</v>
+        <v>15040000</v>
       </c>
       <c r="F63">
-        <v>98880000</v>
+        <v>30080000</v>
       </c>
     </row>
     <row r="64" spans="1:6">
       <c r="A64">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B64" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C64" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D64">
-        <v>2950000</v>
+        <v>910000</v>
       </c>
       <c r="E64">
-        <v>47200000</v>
+        <v>14560000</v>
       </c>
       <c r="F64">
-        <v>94400000</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7">
+        <v>29120000</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="B65" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="C65" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="D65">
-        <v>720000</v>
+        <v>895000</v>
       </c>
       <c r="E65">
-        <v>11520000</v>
+        <v>14320000</v>
       </c>
       <c r="F65">
-        <v>23040000</v>
-      </c>
-      <c r="G65" t="s">
-        <v>135</v>
+        <v>28640000</v>
       </c>
     </row>
     <row r="66" spans="1:6">
       <c r="A66">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="B66" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C66" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="D66">
-        <v>720000</v>
+        <v>875000</v>
       </c>
       <c r="E66">
-        <v>11520000</v>
+        <v>14000000</v>
       </c>
       <c r="F66">
-        <v>23040000</v>
+        <v>28000000</v>
       </c>
     </row>
     <row r="67" spans="1:6">
       <c r="A67">
-        <v>66</v>
+        <v>20</v>
       </c>
       <c r="B67" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C67" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="D67">
-        <v>1155000</v>
+        <v>875000</v>
       </c>
       <c r="E67">
-        <v>18480000</v>
+        <v>14000000</v>
       </c>
       <c r="F67">
-        <v>36960000</v>
+        <v>28000000</v>
       </c>
     </row>
     <row r="68" spans="1:6">
       <c r="A68">
-        <v>67</v>
+        <v>26</v>
       </c>
       <c r="B68" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C68" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D68">
-        <v>940000</v>
+        <v>875000</v>
       </c>
       <c r="E68">
-        <v>15040000</v>
+        <v>14000000</v>
       </c>
       <c r="F68">
-        <v>30080000</v>
+        <v>28000000</v>
       </c>
     </row>
     <row r="69" spans="1:6">
       <c r="A69">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="B69" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C69" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D69">
-        <v>1250000</v>
+        <v>875000</v>
       </c>
       <c r="E69">
-        <v>20000000</v>
+        <v>14000000</v>
       </c>
       <c r="F69">
-        <v>40000000</v>
+        <v>28000000</v>
       </c>
     </row>
     <row r="70" spans="1:6">
       <c r="A70">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="B70" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C70" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D70">
-        <v>940000</v>
+        <v>875000</v>
       </c>
       <c r="E70">
-        <v>15040000</v>
+        <v>14000000</v>
       </c>
       <c r="F70">
-        <v>30080000</v>
+        <v>28000000</v>
       </c>
     </row>
     <row r="71" spans="1:6">
       <c r="A71">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="B71" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="C71" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D71">
-        <v>1100000</v>
+        <v>875000</v>
       </c>
       <c r="E71">
-        <v>17600000</v>
+        <v>14000000</v>
       </c>
       <c r="F71">
-        <v>35200000</v>
+        <v>28000000</v>
       </c>
     </row>
     <row r="72" spans="1:6">
       <c r="A72">
-        <v>71</v>
+        <v>104</v>
       </c>
       <c r="B72" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C72" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D72">
-        <v>940000</v>
+        <v>875000</v>
       </c>
       <c r="E72">
-        <v>15040000</v>
+        <v>14000000</v>
       </c>
       <c r="F72">
-        <v>30080000</v>
+        <v>28000000</v>
       </c>
     </row>
     <row r="73" spans="1:6">
       <c r="A73">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="B73" t="s">
-        <v>150</v>
-      </c>
-      <c r="C73" t="s">
-        <v>151</v>
+        <v>143</v>
+      </c>
+      <c r="C73">
+        <v>128</v>
       </c>
       <c r="D73">
-        <v>1225000</v>
+        <v>875000</v>
       </c>
       <c r="E73">
-        <v>19600000</v>
+        <v>14000000</v>
       </c>
       <c r="F73">
-        <v>39200000</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7">
+        <v>28000000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6">
       <c r="A74">
-        <v>73</v>
+        <v>110</v>
       </c>
       <c r="B74" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C74" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="D74">
-        <v>805000</v>
+        <v>875000</v>
       </c>
       <c r="E74">
-        <v>12880000</v>
+        <v>14000000</v>
       </c>
       <c r="F74">
-        <v>25760000</v>
-      </c>
-      <c r="G74" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7">
+        <v>28000000</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="B75" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C75" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D75">
-        <v>710000</v>
+        <v>845000</v>
       </c>
       <c r="E75">
-        <v>11360000</v>
+        <v>13520000</v>
       </c>
       <c r="F75">
-        <v>22720000</v>
-      </c>
-      <c r="G75" t="s">
-        <v>135</v>
+        <v>27040000</v>
       </c>
     </row>
     <row r="76" spans="1:6">
       <c r="A76">
-        <v>75</v>
+        <v>22</v>
       </c>
       <c r="B76" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C76" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="D76">
-        <v>950000</v>
+        <v>845000</v>
       </c>
       <c r="E76">
-        <v>15200000</v>
+        <v>13520000</v>
       </c>
       <c r="F76">
-        <v>30400000</v>
+        <v>27040000</v>
       </c>
     </row>
     <row r="77" spans="1:6">
       <c r="A77">
-        <v>76</v>
+        <v>41</v>
       </c>
       <c r="B77" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C77" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="D77">
-        <v>1280000</v>
+        <v>845000</v>
       </c>
       <c r="E77">
-        <v>20480000</v>
+        <v>13520000</v>
       </c>
       <c r="F77">
-        <v>40960000</v>
+        <v>27040000</v>
       </c>
     </row>
     <row r="78" spans="1:6">
       <c r="A78">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B78" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C78" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D78">
-        <v>1280000</v>
+        <v>845000</v>
       </c>
       <c r="E78">
-        <v>20480000</v>
+        <v>13520000</v>
       </c>
       <c r="F78">
-        <v>40960000</v>
+        <v>27040000</v>
       </c>
     </row>
     <row r="79" spans="1:6">
       <c r="A79">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B79" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C79" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="D79">
-        <v>1065000</v>
+        <v>845000</v>
       </c>
       <c r="E79">
-        <v>17040000</v>
+        <v>13520000</v>
       </c>
       <c r="F79">
-        <v>34080000</v>
+        <v>27040000</v>
       </c>
     </row>
     <row r="80" spans="1:6">
       <c r="A80">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="B80" t="s">
-        <v>125</v>
+        <v>156</v>
       </c>
       <c r="C80" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="D80">
-        <v>895000</v>
+        <v>845000</v>
       </c>
       <c r="E80">
-        <v>14320000</v>
+        <v>13520000</v>
       </c>
       <c r="F80">
-        <v>28640000</v>
+        <v>27040000</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="B81" t="s">
+        <v>158</v>
+      </c>
+      <c r="C81" t="s">
+        <v>159</v>
+      </c>
+      <c r="D81">
+        <v>845000</v>
+      </c>
+      <c r="E81">
+        <v>13520000</v>
+      </c>
+      <c r="F81">
+        <v>27040000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
+      <c r="A82">
+        <v>97</v>
+      </c>
+      <c r="B82" t="s">
+        <v>160</v>
+      </c>
+      <c r="C82" t="s">
+        <v>161</v>
+      </c>
+      <c r="D82">
+        <v>845000</v>
+      </c>
+      <c r="E82">
+        <v>13520000</v>
+      </c>
+      <c r="F82">
+        <v>27040000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6">
+      <c r="A83">
+        <v>27</v>
+      </c>
+      <c r="B83" t="s">
+        <v>162</v>
+      </c>
+      <c r="C83" t="s">
+        <v>163</v>
+      </c>
+      <c r="D83">
+        <v>825000</v>
+      </c>
+      <c r="E83">
+        <v>13200000</v>
+      </c>
+      <c r="F83">
+        <v>26400000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6">
+      <c r="A84">
+        <v>30</v>
+      </c>
+      <c r="B84" t="s">
+        <v>164</v>
+      </c>
+      <c r="C84" t="s">
         <v>165</v>
       </c>
-      <c r="C81" t="s">
-        <v>166</v>
-      </c>
-      <c r="D81">
-        <v>910000</v>
-      </c>
-      <c r="E81">
-        <v>14560000</v>
-      </c>
-      <c r="F81">
-        <v>29120000</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7">
-      <c r="A82">
-        <v>81</v>
-      </c>
-      <c r="B82" t="s">
-        <v>152</v>
-      </c>
-      <c r="C82" t="s">
-        <v>167</v>
-      </c>
-      <c r="D82">
-        <v>585000</v>
-      </c>
-      <c r="E82">
-        <v>9360000</v>
-      </c>
-      <c r="F82">
-        <v>18720000</v>
-      </c>
-      <c r="G82" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="83" spans="1:7">
-      <c r="A83">
-        <v>82</v>
-      </c>
-      <c r="B83" t="s">
-        <v>168</v>
-      </c>
-      <c r="C83" t="s">
-        <v>169</v>
-      </c>
-      <c r="D83">
-        <v>585000</v>
-      </c>
-      <c r="E83">
-        <v>9360000</v>
-      </c>
-      <c r="F83">
-        <v>18720000</v>
-      </c>
-      <c r="G83" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7">
-      <c r="A84">
-        <v>83</v>
-      </c>
-      <c r="B84" t="s">
-        <v>154</v>
-      </c>
-      <c r="C84" t="s">
-        <v>170</v>
-      </c>
       <c r="D84">
-        <v>585000</v>
+        <v>825000</v>
       </c>
       <c r="E84">
-        <v>9360000</v>
+        <v>13200000</v>
       </c>
       <c r="F84">
-        <v>18720000</v>
-      </c>
-      <c r="G84" t="s">
-        <v>135</v>
+        <v>26400000</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -3425,10 +3395,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>156</v>
+        <v>86</v>
       </c>
       <c r="C85" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D85">
         <v>825000</v>
@@ -3445,10 +3415,10 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="C86" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D86">
         <v>825000</v>
@@ -3460,267 +3430,267 @@
         <v>26400000</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:7">
       <c r="A87">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="B87" t="s">
-        <v>158</v>
+        <v>169</v>
       </c>
       <c r="C87" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D87">
-        <v>1155000</v>
+        <v>805000</v>
       </c>
       <c r="E87">
-        <v>18480000</v>
+        <v>12880000</v>
       </c>
       <c r="F87">
-        <v>36960000</v>
+        <v>25760000</v>
+      </c>
+      <c r="G87" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88">
-        <v>87</v>
+        <v>5</v>
       </c>
       <c r="B88" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C88" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D88">
-        <v>1155000</v>
+        <v>785000</v>
       </c>
       <c r="E88">
-        <v>18480000</v>
+        <v>12560000</v>
       </c>
       <c r="F88">
-        <v>36960000</v>
+        <v>25120000</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89">
-        <v>88</v>
+        <v>8</v>
       </c>
       <c r="B89" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C89" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D89">
-        <v>940000</v>
+        <v>785000</v>
       </c>
       <c r="E89">
-        <v>15040000</v>
+        <v>12560000</v>
       </c>
       <c r="F89">
-        <v>30080000</v>
+        <v>25120000</v>
       </c>
     </row>
     <row r="90" spans="1:6">
       <c r="A90">
-        <v>89</v>
+        <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C90" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D90">
-        <v>940000</v>
+        <v>785000</v>
       </c>
       <c r="E90">
-        <v>15040000</v>
+        <v>12560000</v>
       </c>
       <c r="F90">
-        <v>30080000</v>
+        <v>25120000</v>
       </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="B91" t="s">
-        <v>160</v>
+        <v>178</v>
       </c>
       <c r="C91" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D91">
-        <v>1155000</v>
+        <v>785000</v>
       </c>
       <c r="E91">
-        <v>18480000</v>
+        <v>12560000</v>
       </c>
       <c r="F91">
-        <v>36960000</v>
+        <v>25120000</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92">
-        <v>91</v>
+        <v>12</v>
       </c>
       <c r="B92" t="s">
-        <v>162</v>
+        <v>180</v>
       </c>
       <c r="C92" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D92">
-        <v>940000</v>
+        <v>785000</v>
       </c>
       <c r="E92">
-        <v>15040000</v>
+        <v>12560000</v>
       </c>
       <c r="F92">
-        <v>30080000</v>
+        <v>25120000</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93">
-        <v>92</v>
+        <v>16</v>
       </c>
       <c r="B93" t="s">
+        <v>182</v>
+      </c>
+      <c r="C93" t="s">
         <v>183</v>
       </c>
-      <c r="C93" t="s">
-        <v>184</v>
-      </c>
       <c r="D93">
-        <v>940000</v>
+        <v>785000</v>
       </c>
       <c r="E93">
-        <v>15040000</v>
+        <v>12560000</v>
       </c>
       <c r="F93">
-        <v>30080000</v>
+        <v>25120000</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94">
-        <v>93</v>
+        <v>17</v>
       </c>
       <c r="B94" t="s">
+        <v>184</v>
+      </c>
+      <c r="C94" t="s">
         <v>185</v>
       </c>
-      <c r="C94" t="s">
-        <v>186</v>
-      </c>
       <c r="D94">
-        <v>585000</v>
+        <v>785000</v>
       </c>
       <c r="E94">
-        <v>9360000</v>
+        <v>12560000</v>
       </c>
       <c r="F94">
-        <v>18720000</v>
+        <v>25120000</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="B95" t="s">
+        <v>186</v>
+      </c>
+      <c r="C95" t="s">
         <v>187</v>
       </c>
-      <c r="C95">
-        <v>125</v>
-      </c>
       <c r="D95">
-        <v>940000</v>
+        <v>785000</v>
       </c>
       <c r="E95">
-        <v>15040000</v>
+        <v>12560000</v>
       </c>
       <c r="F95">
-        <v>30080000</v>
+        <v>25120000</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96">
-        <v>95</v>
+        <v>19</v>
       </c>
       <c r="B96" t="s">
         <v>188</v>
       </c>
-      <c r="C96">
-        <v>127</v>
+      <c r="C96" t="s">
+        <v>189</v>
       </c>
       <c r="D96">
-        <v>940000</v>
+        <v>785000</v>
       </c>
       <c r="E96">
-        <v>15040000</v>
+        <v>12560000</v>
       </c>
       <c r="F96">
-        <v>30080000</v>
+        <v>25120000</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97">
-        <v>96</v>
+        <v>24</v>
       </c>
       <c r="B97" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C97" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D97">
-        <v>940000</v>
+        <v>785000</v>
       </c>
       <c r="E97">
-        <v>15040000</v>
+        <v>12560000</v>
       </c>
       <c r="F97">
-        <v>30080000</v>
+        <v>25120000</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="B98" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C98" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D98">
-        <v>845000</v>
+        <v>785000</v>
       </c>
       <c r="E98">
-        <v>13520000</v>
+        <v>12560000</v>
       </c>
       <c r="F98">
-        <v>27040000</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7">
+        <v>25120000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6">
       <c r="A99">
-        <v>98</v>
+        <v>35</v>
       </c>
       <c r="B99" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C99" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D99">
-        <v>585000</v>
+        <v>785000</v>
       </c>
       <c r="E99">
-        <v>9360000</v>
+        <v>12560000</v>
       </c>
       <c r="F99">
-        <v>18720000</v>
-      </c>
-      <c r="G99" t="s">
-        <v>135</v>
+        <v>25120000</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -3728,10 +3698,10 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C100" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D100">
         <v>785000</v>
@@ -3743,32 +3713,29 @@
         <v>25120000</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:6">
       <c r="A101">
-        <v>100</v>
+        <v>60</v>
       </c>
       <c r="B101" t="s">
-        <v>197</v>
+        <v>127</v>
       </c>
       <c r="C101" t="s">
         <v>198</v>
       </c>
       <c r="D101">
-        <v>585000</v>
+        <v>770000</v>
       </c>
       <c r="E101">
-        <v>9360000</v>
+        <v>12320000</v>
       </c>
       <c r="F101">
-        <v>18720000</v>
-      </c>
-      <c r="G101" t="s">
-        <v>135</v>
+        <v>24640000</v>
       </c>
     </row>
     <row r="102" spans="1:7">
       <c r="A102">
-        <v>101</v>
+        <v>64</v>
       </c>
       <c r="B102" t="s">
         <v>199</v>
@@ -3777,21 +3744,21 @@
         <v>200</v>
       </c>
       <c r="D102">
-        <v>585000</v>
+        <v>720000</v>
       </c>
       <c r="E102">
-        <v>9360000</v>
+        <v>11520000</v>
       </c>
       <c r="F102">
-        <v>18720000</v>
+        <v>23040000</v>
       </c>
       <c r="G102" t="s">
-        <v>135</v>
+        <v>171</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="B103" t="s">
         <v>201</v>
@@ -3800,18 +3767,18 @@
         <v>202</v>
       </c>
       <c r="D103">
-        <v>940000</v>
+        <v>720000</v>
       </c>
       <c r="E103">
-        <v>15040000</v>
+        <v>11520000</v>
       </c>
       <c r="F103">
-        <v>30080000</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6">
+        <v>23040000</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="B104" t="s">
         <v>203</v>
@@ -3820,18 +3787,21 @@
         <v>204</v>
       </c>
       <c r="D104">
-        <v>1100000</v>
+        <v>710000</v>
       </c>
       <c r="E104">
-        <v>17600000</v>
+        <v>11360000</v>
       </c>
       <c r="F104">
-        <v>35200000</v>
+        <v>22720000</v>
+      </c>
+      <c r="G104" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="B105" t="s">
         <v>205</v>
@@ -3840,18 +3810,18 @@
         <v>206</v>
       </c>
       <c r="D105">
-        <v>875000</v>
+        <v>700000</v>
       </c>
       <c r="E105">
-        <v>14000000</v>
+        <v>11200000</v>
       </c>
       <c r="F105">
-        <v>28000000</v>
+        <v>22400000</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106">
-        <v>105</v>
+        <v>32</v>
       </c>
       <c r="B106" t="s">
         <v>207</v>
@@ -3860,18 +3830,18 @@
         <v>208</v>
       </c>
       <c r="D106">
-        <v>940000</v>
+        <v>700000</v>
       </c>
       <c r="E106">
-        <v>15040000</v>
+        <v>11200000</v>
       </c>
       <c r="F106">
-        <v>30080000</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6">
+        <v>22400000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107">
-        <v>106</v>
+        <v>54</v>
       </c>
       <c r="B107" t="s">
         <v>209</v>
@@ -3880,98 +3850,113 @@
         <v>210</v>
       </c>
       <c r="D107">
-        <v>1035000</v>
+        <v>680000</v>
       </c>
       <c r="E107">
-        <v>16560000</v>
+        <v>10880000</v>
       </c>
       <c r="F107">
-        <v>33120000</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6">
+        <v>21760000</v>
+      </c>
+      <c r="G107" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="B108" t="s">
+        <v>212</v>
+      </c>
+      <c r="C108" t="s">
+        <v>213</v>
+      </c>
+      <c r="D108">
+        <v>680000</v>
+      </c>
+      <c r="E108">
+        <v>10880000</v>
+      </c>
+      <c r="F108">
+        <v>21760000</v>
+      </c>
+      <c r="G108" t="s">
         <v>211</v>
       </c>
-      <c r="C108" t="s">
-        <v>212</v>
-      </c>
-      <c r="D108">
-        <v>940000</v>
-      </c>
-      <c r="E108">
-        <v>15040000</v>
-      </c>
-      <c r="F108">
-        <v>30080000</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6">
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="B109" t="s">
-        <v>213</v>
-      </c>
-      <c r="C109">
-        <v>128</v>
+        <v>169</v>
+      </c>
+      <c r="C109" t="s">
+        <v>214</v>
       </c>
       <c r="D109">
-        <v>875000</v>
+        <v>585000</v>
       </c>
       <c r="E109">
-        <v>14000000</v>
+        <v>9360000</v>
       </c>
       <c r="F109">
-        <v>28000000</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6">
+        <v>18720000</v>
+      </c>
+      <c r="G109" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="B110" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C110" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D110">
-        <v>1035000</v>
+        <v>585000</v>
       </c>
       <c r="E110">
-        <v>16560000</v>
+        <v>9360000</v>
       </c>
       <c r="F110">
-        <v>33120000</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6">
+        <v>18720000</v>
+      </c>
+      <c r="G110" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="B111" t="s">
-        <v>216</v>
+        <v>203</v>
       </c>
       <c r="C111" t="s">
         <v>217</v>
       </c>
       <c r="D111">
-        <v>875000</v>
+        <v>585000</v>
       </c>
       <c r="E111">
-        <v>14000000</v>
+        <v>9360000</v>
       </c>
       <c r="F111">
-        <v>28000000</v>
+        <v>18720000</v>
+      </c>
+      <c r="G111" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112">
-        <v>111</v>
+        <v>93</v>
       </c>
       <c r="B112" t="s">
         <v>218</v>
@@ -3980,71 +3965,86 @@
         <v>219</v>
       </c>
       <c r="D112">
-        <v>1250000</v>
+        <v>585000</v>
       </c>
       <c r="E112">
-        <v>20000000</v>
-      </c>
-      <c r="F112" s="2">
-        <v>40000000</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6">
+        <v>9360000</v>
+      </c>
+      <c r="F112">
+        <v>18720000</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113">
-        <v>112</v>
-      </c>
-      <c r="B113" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B113" t="s">
         <v>220</v>
       </c>
-      <c r="C113" s="3" t="s">
+      <c r="C113" t="s">
         <v>221</v>
       </c>
-      <c r="D113" s="3"/>
+      <c r="D113">
+        <v>585000</v>
+      </c>
       <c r="E113">
-        <v>32000000</v>
-      </c>
-      <c r="F113" s="3">
-        <v>64000000</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6">
+        <v>9360000</v>
+      </c>
+      <c r="F113">
+        <v>18720000</v>
+      </c>
+      <c r="G113" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
       <c r="A114">
-        <v>113</v>
-      </c>
-      <c r="B114" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B114" t="s">
         <v>222</v>
       </c>
-      <c r="C114" s="3" t="s">
+      <c r="C114" t="s">
         <v>223</v>
       </c>
-      <c r="D114" s="3"/>
+      <c r="D114">
+        <v>585000</v>
+      </c>
       <c r="E114">
-        <v>32000000</v>
-      </c>
-      <c r="F114" s="3">
-        <v>64000000</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6">
+        <v>9360000</v>
+      </c>
+      <c r="F114">
+        <v>18720000</v>
+      </c>
+      <c r="G114" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
       <c r="A115">
-        <v>114</v>
-      </c>
-      <c r="B115" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B115" t="s">
         <v>224</v>
       </c>
-      <c r="C115" s="3" t="s">
+      <c r="C115" t="s">
         <v>225</v>
       </c>
-      <c r="D115" s="3"/>
+      <c r="D115">
+        <v>585000</v>
+      </c>
       <c r="E115">
-        <v>32000000</v>
-      </c>
-      <c r="F115" s="3">
-        <v>64000000</v>
+        <v>9360000</v>
+      </c>
+      <c r="F115">
+        <v>18720000</v>
+      </c>
+      <c r="G115" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="116" spans="6:6">
-      <c r="F116" s="2"/>
+      <c r="F116" s="3"/>
     </row>
     <row r="119" spans="8:8">
       <c r="H119" s="4"/>
@@ -4053,8 +4053,8 @@
       <c r="H120" s="4"/>
     </row>
   </sheetData>
-  <sortState ref="A2:G112">
-    <sortCondition ref="A2"/>
+  <sortState ref="A2:G115">
+    <sortCondition ref="F2" descending="1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>